<commit_message>
31.08.19 today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Requisition of Tulip-2/29 August Requisition of Tulip-2.xlsx
+++ b/August/Others/Requisition of Tulip-2/29 August Requisition of Tulip-2.xlsx
@@ -1004,10 +1004,10 @@
   <dimension ref="A1:BC96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E84" sqref="E84"/>
+      <selection pane="bottomRight" activeCell="I86" sqref="I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>

</xml_diff>